<commit_message>
BR Class 380 Desiro complete
</commit_message>
<xml_diff>
--- a/docs/New Template Calculations.xlsx
+++ b/docs/New Template Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BRTrains2-Extended\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC927EE-8C02-4DF9-848F-F0EAF591C4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE93C41-FD8B-419B-A39B-FEBC8AF73FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{D51931E5-81BC-4C5B-8C55-7A4B86E09E95}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="698" xr2:uid="{D51931E5-81BC-4C5B-8C55-7A4B86E09E95}"/>
   </bookViews>
   <sheets>
     <sheet name="1x" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="286">
   <si>
     <t>Horizontal</t>
   </si>
@@ -892,6 +892,9 @@
   </si>
   <si>
     <t>LMS Fowler 4P Compound</t>
+  </si>
+  <si>
+    <t>Voxel</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1156,12 +1159,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -1498,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C473DBD1-BF4E-4659-B175-DA8950A0E94D}">
   <dimension ref="A1:AB48"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:N14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,6 +1555,9 @@
       <c r="D2" s="27" t="s">
         <v>27</v>
       </c>
+      <c r="E2" s="45" t="s">
+        <v>285</v>
+      </c>
       <c r="F2" s="25" t="s">
         <v>4</v>
       </c>
@@ -1887,6 +1894,9 @@
       <c r="D6" s="11">
         <v>22</v>
       </c>
+      <c r="E6">
+        <v>66</v>
+      </c>
       <c r="F6" s="9">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1975,6 +1985,9 @@
       <c r="D7" s="8">
         <v>27.5</v>
       </c>
+      <c r="E7" s="1">
+        <v>82</v>
+      </c>
       <c r="F7" s="6">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -2063,6 +2076,9 @@
       <c r="D8" s="11">
         <v>33</v>
       </c>
+      <c r="E8">
+        <v>98</v>
+      </c>
       <c r="F8" s="9">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -2151,6 +2167,9 @@
       <c r="D9" s="8">
         <v>38.5</v>
       </c>
+      <c r="E9" s="1">
+        <v>114</v>
+      </c>
       <c r="F9" s="6">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -2238,6 +2257,9 @@
       </c>
       <c r="D10" s="11">
         <v>44</v>
+      </c>
+      <c r="E10">
+        <v>132</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="1"/>
@@ -2325,7 +2347,9 @@
       <c r="D11" s="8">
         <v>49.5</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>148</v>
+      </c>
       <c r="F11" s="6">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -2416,6 +2440,9 @@
       <c r="D12" s="11">
         <v>55</v>
       </c>
+      <c r="E12">
+        <v>164</v>
+      </c>
       <c r="F12" s="9">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2502,7 +2529,9 @@
       <c r="D13" s="8">
         <v>60.5</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1">
+        <v>180</v>
+      </c>
       <c r="F13" s="6">
         <f>C13</f>
         <v>44</v>
@@ -2595,6 +2624,9 @@
       <c r="D14" s="11">
         <v>66</v>
       </c>
+      <c r="E14">
+        <v>198</v>
+      </c>
       <c r="F14" s="9">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -2681,7 +2713,9 @@
       <c r="D15" s="8">
         <v>71.5</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>214</v>
+      </c>
       <c r="F15" s="6">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -2771,6 +2805,9 @@
       <c r="D16" s="11">
         <v>77</v>
       </c>
+      <c r="E16">
+        <v>230</v>
+      </c>
       <c r="F16" s="9">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2857,7 +2894,9 @@
       <c r="D17" s="8">
         <v>82.5</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>246</v>
+      </c>
       <c r="F17" s="6">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -2946,6 +2985,9 @@
       </c>
       <c r="D18" s="14">
         <v>88</v>
+      </c>
+      <c r="E18">
+        <v>255</v>
       </c>
       <c r="F18" s="12">
         <f t="shared" si="1"/>
@@ -7824,7 +7866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCDE093-BF87-48D4-BE7D-AFEA8C3CA6A0}">
   <dimension ref="A1:M211"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2835" ySplit="765" topLeftCell="G180" activePane="bottomRight"/>
       <selection activeCell="B2" sqref="A2:XFD2"/>
       <selection pane="topRight" activeCell="E1" sqref="E1:E1048576"/>
@@ -7889,7 +7931,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="36">
@@ -7897,49 +7939,49 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
+      <c r="A3" s="44"/>
       <c r="B3" s="36">
         <v>1851</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="36">
         <v>1852</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="36">
         <v>1853</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="36">
         <v>1854</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="36">
         <v>1855</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="36">
         <v>1856</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="36">
         <v>1857</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="36">
         <v>1858</v>
       </c>
@@ -7948,7 +7990,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="36">
         <v>1859</v>
       </c>
@@ -7957,55 +7999,55 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="36">
         <v>1860</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="36">
         <v>1861</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="36">
         <v>1862</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="36">
         <v>1863</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="36">
         <v>1864</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="36">
         <v>1865</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="36">
         <v>1866</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="36">
         <v>1867</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="36">
         <v>1868</v>
       </c>
@@ -8014,13 +8056,13 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="36">
         <v>1869</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="36">
         <v>1870</v>
       </c>
@@ -8029,13 +8071,13 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="36">
         <v>1871</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="36">
         <v>1872</v>
       </c>
@@ -8044,7 +8086,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="36">
         <v>1873</v>
       </c>
@@ -8053,13 +8095,13 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="36">
         <v>1874</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="36">
         <v>1875</v>
       </c>
@@ -8068,37 +8110,37 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="36">
         <v>1876</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="43"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="36">
         <v>1877</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="43"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="36">
         <v>1878</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="36">
         <v>1879</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="36">
         <v>1880</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="36">
         <v>1881</v>
       </c>
@@ -8107,7 +8149,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="36">
         <v>1882</v>
       </c>
@@ -8119,7 +8161,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="36">
         <v>1883</v>
       </c>
@@ -8128,7 +8170,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="36">
         <v>1884</v>
       </c>
@@ -8137,13 +8179,13 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="36">
         <v>1885</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="36">
         <v>1886</v>
       </c>
@@ -8152,37 +8194,37 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="36">
         <v>1887</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
+      <c r="A40" s="44"/>
       <c r="B40" s="36">
         <v>1888</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
+      <c r="A41" s="44"/>
       <c r="B41" s="36">
         <v>1889</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="36">
         <v>1890</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="43"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="36">
         <v>1891</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
+      <c r="A44" s="44"/>
       <c r="B44" s="36">
         <v>1892</v>
       </c>
@@ -8191,19 +8233,19 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="43"/>
+      <c r="A45" s="44"/>
       <c r="B45" s="36">
         <v>1893</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="43"/>
+      <c r="A46" s="44"/>
       <c r="B46" s="36">
         <v>1894</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="43"/>
+      <c r="A47" s="44"/>
       <c r="B47" s="36">
         <v>1895</v>
       </c>
@@ -8212,7 +8254,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="43"/>
+      <c r="A48" s="44"/>
       <c r="B48" s="36">
         <v>1896</v>
       </c>
@@ -8221,13 +8263,13 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="43"/>
+      <c r="A49" s="44"/>
       <c r="C49" s="31" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="43"/>
+      <c r="A50" s="44"/>
       <c r="B50" s="36">
         <v>1897</v>
       </c>
@@ -8236,25 +8278,25 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="43"/>
+      <c r="A51" s="44"/>
       <c r="F51" s="31" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="43"/>
+      <c r="A52" s="44"/>
       <c r="B52" s="36">
         <v>1898</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="43"/>
+      <c r="A53" s="44"/>
       <c r="B53" s="36">
         <v>1899</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="43" t="s">
+      <c r="A54" s="44" t="s">
         <v>56</v>
       </c>
       <c r="B54" s="36">
@@ -8268,7 +8310,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="43"/>
+      <c r="A55" s="44"/>
       <c r="B55" s="36">
         <v>1901</v>
       </c>
@@ -8277,7 +8319,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="43"/>
+      <c r="A56" s="44"/>
       <c r="B56" s="36">
         <v>1902</v>
       </c>
@@ -8289,13 +8331,13 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="43"/>
+      <c r="A57" s="44"/>
       <c r="G57" s="31" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="43"/>
+      <c r="A58" s="44"/>
       <c r="B58" s="36">
         <v>1903</v>
       </c>
@@ -8310,13 +8352,13 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="43"/>
+      <c r="A59" s="44"/>
       <c r="D59" s="31" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="43"/>
+      <c r="A60" s="44"/>
       <c r="B60" s="36">
         <v>1904</v>
       </c>
@@ -8328,13 +8370,13 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="43"/>
+      <c r="A61" s="44"/>
       <c r="B61" s="36">
         <v>1905</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="43"/>
+      <c r="A62" s="44"/>
       <c r="B62" s="36">
         <v>1906</v>
       </c>
@@ -8346,7 +8388,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="43"/>
+      <c r="A63" s="44"/>
       <c r="B63" s="36">
         <v>1907</v>
       </c>
@@ -8355,7 +8397,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="43"/>
+      <c r="A64" s="44"/>
       <c r="B64" s="36">
         <v>1908</v>
       </c>
@@ -8364,7 +8406,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="43"/>
+      <c r="A65" s="44"/>
       <c r="B65" s="36">
         <v>1909</v>
       </c>
@@ -8373,13 +8415,13 @@
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" s="43"/>
+      <c r="A66" s="44"/>
       <c r="B66" s="36">
         <v>1910</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" s="43"/>
+      <c r="A67" s="44"/>
       <c r="B67" s="36">
         <v>1911</v>
       </c>
@@ -8397,13 +8439,13 @@
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="43"/>
+      <c r="A68" s="44"/>
       <c r="B68" s="36">
         <v>1912</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="43"/>
+      <c r="A69" s="44"/>
       <c r="B69" s="36">
         <v>1913</v>
       </c>
@@ -8418,7 +8460,7 @@
       </c>
     </row>
     <row r="70" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="43"/>
+      <c r="A70" s="44"/>
       <c r="B70" s="36">
         <v>1914</v>
       </c>
@@ -8436,7 +8478,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" s="43"/>
+      <c r="A71" s="44"/>
       <c r="B71" s="36">
         <v>1915</v>
       </c>
@@ -8445,13 +8487,13 @@
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="43"/>
+      <c r="A72" s="44"/>
       <c r="B72" s="36">
         <v>1916</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="43"/>
+      <c r="A73" s="44"/>
       <c r="B73" s="36">
         <v>1917</v>
       </c>
@@ -8460,7 +8502,7 @@
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" s="43"/>
+      <c r="A74" s="44"/>
       <c r="B74" s="36">
         <v>1918</v>
       </c>
@@ -8472,7 +8514,7 @@
       </c>
     </row>
     <row r="75" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="43"/>
+      <c r="A75" s="44"/>
       <c r="B75" s="36">
         <v>1919</v>
       </c>
@@ -8490,7 +8532,7 @@
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="43"/>
+      <c r="A76" s="44"/>
       <c r="B76" s="36">
         <v>1920</v>
       </c>
@@ -8499,7 +8541,7 @@
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77" s="43" t="s">
+      <c r="A77" s="44" t="s">
         <v>57</v>
       </c>
       <c r="B77" s="36">
@@ -8507,7 +8549,7 @@
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78" s="43"/>
+      <c r="A78" s="44"/>
       <c r="B78" s="36">
         <v>1922</v>
       </c>
@@ -8516,7 +8558,7 @@
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" s="43"/>
+      <c r="A79" s="44"/>
       <c r="B79" s="36">
         <v>1923</v>
       </c>
@@ -8528,7 +8570,7 @@
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" s="43"/>
+      <c r="A80" s="44"/>
       <c r="B80" s="36">
         <v>1924</v>
       </c>
@@ -8543,13 +8585,13 @@
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" s="43"/>
+      <c r="A81" s="44"/>
       <c r="B81" s="36">
         <v>1925</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" s="43"/>
+      <c r="A82" s="44"/>
       <c r="B82" s="36">
         <v>1926</v>
       </c>
@@ -8561,8 +8603,8 @@
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" s="43"/>
-      <c r="B83" s="43">
+      <c r="A83" s="44"/>
+      <c r="B83" s="44">
         <v>1927</v>
       </c>
       <c r="C83" s="31" t="s">
@@ -8579,8 +8621,8 @@
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="43"/>
-      <c r="B84" s="43"/>
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
       <c r="C84" s="31" t="s">
         <v>92</v>
       </c>
@@ -8589,7 +8631,7 @@
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="43"/>
+      <c r="A85" s="44"/>
       <c r="B85" s="36">
         <v>1928</v>
       </c>
@@ -8607,8 +8649,8 @@
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" s="43"/>
-      <c r="B86" s="43">
+      <c r="A86" s="44"/>
+      <c r="B86" s="44">
         <v>1929</v>
       </c>
       <c r="C86" s="31" t="s">
@@ -8625,14 +8667,14 @@
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" s="43"/>
-      <c r="B87" s="43"/>
+      <c r="A87" s="44"/>
+      <c r="B87" s="44"/>
       <c r="C87" s="31" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" s="43"/>
+      <c r="A88" s="44"/>
       <c r="B88" s="36">
         <v>1930</v>
       </c>
@@ -8647,7 +8689,7 @@
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="43"/>
+      <c r="A89" s="44"/>
       <c r="B89" s="36">
         <v>1931</v>
       </c>
@@ -8656,7 +8698,7 @@
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" s="43"/>
+      <c r="A90" s="44"/>
       <c r="B90" s="36">
         <v>1932</v>
       </c>
@@ -8668,19 +8710,19 @@
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A91" s="43"/>
+      <c r="A91" s="44"/>
       <c r="L91" s="31" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A92" s="43"/>
+      <c r="A92" s="44"/>
       <c r="L92" s="31" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A93" s="43"/>
+      <c r="A93" s="44"/>
       <c r="B93" s="36">
         <v>1933</v>
       </c>
@@ -8692,10 +8734,10 @@
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A94" s="43"/>
+      <c r="A94" s="44"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A95" s="43"/>
+      <c r="A95" s="44"/>
       <c r="B95" s="36">
         <v>1934</v>
       </c>
@@ -8716,7 +8758,7 @@
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" s="43"/>
+      <c r="A96" s="44"/>
       <c r="B96" s="36">
         <v>1935</v>
       </c>
@@ -8731,8 +8773,8 @@
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A97" s="43"/>
-      <c r="B97" s="43">
+      <c r="A97" s="44"/>
+      <c r="B97" s="44">
         <v>1936</v>
       </c>
       <c r="C97" s="31" t="s">
@@ -8746,8 +8788,8 @@
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A98" s="43"/>
-      <c r="B98" s="43"/>
+      <c r="A98" s="44"/>
+      <c r="B98" s="44"/>
       <c r="C98" s="31" t="s">
         <v>127</v>
       </c>
@@ -8756,7 +8798,7 @@
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A99" s="43"/>
+      <c r="A99" s="44"/>
       <c r="B99" s="36">
         <v>1937</v>
       </c>
@@ -8771,28 +8813,28 @@
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A100" s="43"/>
+      <c r="A100" s="44"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A101" s="43"/>
+      <c r="A101" s="44"/>
       <c r="B101" s="36">
         <v>1938</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A102" s="43"/>
+      <c r="A102" s="44"/>
       <c r="B102" s="36">
         <v>1939</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A103" s="43"/>
+      <c r="A103" s="44"/>
       <c r="B103" s="36">
         <v>1940</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A104" s="43"/>
+      <c r="A104" s="44"/>
       <c r="B104" s="36">
         <v>1941</v>
       </c>
@@ -8807,19 +8849,19 @@
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A105" s="43"/>
+      <c r="A105" s="44"/>
       <c r="E105" s="31" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A106" s="43"/>
+      <c r="A106" s="44"/>
       <c r="E106" s="31" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A107" s="43"/>
+      <c r="A107" s="44"/>
       <c r="B107" s="36">
         <v>1942</v>
       </c>
@@ -8837,7 +8879,7 @@
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A108" s="43"/>
+      <c r="A108" s="44"/>
       <c r="B108" s="36">
         <v>1943</v>
       </c>
@@ -8855,7 +8897,7 @@
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A109" s="43"/>
+      <c r="A109" s="44"/>
       <c r="B109" s="36">
         <v>1944</v>
       </c>
@@ -8867,7 +8909,7 @@
       </c>
     </row>
     <row r="110" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="43"/>
+      <c r="A110" s="44"/>
       <c r="B110" s="36">
         <v>1945</v>
       </c>
@@ -8876,13 +8918,13 @@
       </c>
     </row>
     <row r="111" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A111" s="43"/>
+      <c r="A111" s="44"/>
       <c r="C111" s="31" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A112" s="43"/>
+      <c r="A112" s="44"/>
       <c r="B112" s="36">
         <v>1946</v>
       </c>
@@ -8897,7 +8939,7 @@
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A113" s="43"/>
+      <c r="A113" s="44"/>
       <c r="B113" s="36">
         <v>1947</v>
       </c>
@@ -8909,7 +8951,7 @@
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" s="43" t="s">
+      <c r="A114" s="44" t="s">
         <v>58</v>
       </c>
       <c r="B114" s="36">
@@ -8932,7 +8974,7 @@
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A115" s="43"/>
+      <c r="A115" s="44"/>
       <c r="C115" s="31" t="s">
         <v>147</v>
       </c>
@@ -8944,7 +8986,7 @@
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A116" s="43"/>
+      <c r="A116" s="44"/>
       <c r="E116" s="31" t="s">
         <v>151</v>
       </c>
@@ -8953,13 +8995,13 @@
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A117" s="43"/>
+      <c r="A117" s="44"/>
       <c r="F117" s="31" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A118" s="43"/>
+      <c r="A118" s="44"/>
       <c r="B118" s="36">
         <v>1949</v>
       </c>
@@ -8968,13 +9010,13 @@
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A119" s="43"/>
+      <c r="A119" s="44"/>
       <c r="B119" s="36">
         <v>1950</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A120" s="43"/>
+      <c r="A120" s="44"/>
       <c r="B120" s="36">
         <v>1951</v>
       </c>
@@ -8983,13 +9025,13 @@
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A121" s="43"/>
+      <c r="A121" s="44"/>
       <c r="B121" s="36">
         <v>1952</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A122" s="43"/>
+      <c r="A122" s="44"/>
       <c r="B122" s="36">
         <v>1953</v>
       </c>
@@ -8998,13 +9040,13 @@
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A123" s="43"/>
+      <c r="A123" s="44"/>
       <c r="B123" s="36">
         <v>1954</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A124" s="43"/>
+      <c r="A124" s="44"/>
       <c r="B124" s="36">
         <v>1955</v>
       </c>
@@ -9013,16 +9055,16 @@
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A125" s="43"/>
+      <c r="A125" s="44"/>
       <c r="C125" s="31" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A126" s="43"/>
+      <c r="A126" s="44"/>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A127" s="43" t="s">
+      <c r="A127" s="44" t="s">
         <v>59</v>
       </c>
       <c r="B127" s="36">
@@ -9033,7 +9075,7 @@
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A128" s="43"/>
+      <c r="A128" s="44"/>
       <c r="B128" s="36">
         <v>1957</v>
       </c>
@@ -9045,7 +9087,7 @@
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A129" s="43"/>
+      <c r="A129" s="44"/>
       <c r="B129" s="36">
         <v>1958</v>
       </c>
@@ -9057,13 +9099,13 @@
       </c>
     </row>
     <row r="130" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A130" s="43"/>
+      <c r="A130" s="44"/>
       <c r="C130" s="31" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="131" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A131" s="43"/>
+      <c r="A131" s="44"/>
       <c r="B131" s="36">
         <v>1959</v>
       </c>
@@ -9075,13 +9117,13 @@
       </c>
     </row>
     <row r="132" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="43"/>
+      <c r="A132" s="44"/>
       <c r="J132" s="31" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="133" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A133" s="43"/>
+      <c r="A133" s="44"/>
       <c r="B133" s="36">
         <v>1960</v>
       </c>
@@ -9096,14 +9138,14 @@
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A134" s="43"/>
+      <c r="A134" s="44"/>
       <c r="D134" s="31" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="135" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" s="43"/>
-      <c r="B135" s="43">
+      <c r="A135" s="44"/>
+      <c r="B135" s="44">
         <v>1961</v>
       </c>
       <c r="C135" s="31" t="s">
@@ -9114,28 +9156,28 @@
       </c>
     </row>
     <row r="136" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A136" s="43"/>
-      <c r="B136" s="43"/>
+      <c r="A136" s="44"/>
+      <c r="B136" s="44"/>
       <c r="C136" s="31" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A137" s="43"/>
-      <c r="B137" s="43"/>
+      <c r="A137" s="44"/>
+      <c r="B137" s="44"/>
       <c r="C137" s="31" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A138" s="43"/>
-      <c r="B138" s="43"/>
+      <c r="A138" s="44"/>
+      <c r="B138" s="44"/>
       <c r="C138" s="31" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A139" s="43"/>
+      <c r="A139" s="44"/>
       <c r="B139" s="36">
         <v>1962</v>
       </c>
@@ -9144,7 +9186,7 @@
       </c>
     </row>
     <row r="140" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A140" s="43"/>
+      <c r="A140" s="44"/>
       <c r="B140" s="36">
         <v>1963</v>
       </c>
@@ -9153,7 +9195,7 @@
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A141" s="43"/>
+      <c r="A141" s="44"/>
       <c r="B141" s="36">
         <v>1964</v>
       </c>
@@ -9162,7 +9204,7 @@
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A142" s="43"/>
+      <c r="A142" s="44"/>
       <c r="B142" s="36">
         <v>1965</v>
       </c>
@@ -9174,7 +9216,7 @@
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A143" s="43"/>
+      <c r="A143" s="44"/>
       <c r="B143" s="36">
         <v>1966</v>
       </c>
@@ -9183,13 +9225,13 @@
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A144" s="43"/>
+      <c r="A144" s="44"/>
       <c r="L144" s="31" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A145" s="43"/>
+      <c r="A145" s="44"/>
       <c r="B145" s="36">
         <v>1967</v>
       </c>
@@ -9198,25 +9240,25 @@
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A146" s="43"/>
+      <c r="A146" s="44"/>
       <c r="B146" s="36">
         <v>1968</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A147" s="43"/>
+      <c r="A147" s="44"/>
       <c r="B147" s="36">
         <v>1969</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A148" s="43"/>
+      <c r="A148" s="44"/>
       <c r="B148" s="36">
         <v>1970</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A149" s="43" t="s">
+      <c r="A149" s="44" t="s">
         <v>60</v>
       </c>
       <c r="B149" s="36">
@@ -9224,7 +9266,7 @@
       </c>
     </row>
     <row r="150" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="43"/>
+      <c r="A150" s="44"/>
       <c r="B150" s="36">
         <v>1972</v>
       </c>
@@ -9236,19 +9278,19 @@
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A151" s="43"/>
+      <c r="A151" s="44"/>
       <c r="B151" s="36">
         <v>1973</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A152" s="43"/>
+      <c r="A152" s="44"/>
       <c r="B152" s="36">
         <v>1974</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A153" s="43"/>
+      <c r="A153" s="44"/>
       <c r="B153" s="36">
         <v>1975</v>
       </c>
@@ -9257,13 +9299,13 @@
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A154" s="43"/>
+      <c r="A154" s="44"/>
       <c r="J154" s="31" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A155" s="43"/>
+      <c r="A155" s="44"/>
       <c r="B155" s="36">
         <v>1976</v>
       </c>
@@ -9272,19 +9314,19 @@
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A156" s="43"/>
+      <c r="A156" s="44"/>
       <c r="B156" s="36">
         <v>1977</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A157" s="43"/>
+      <c r="A157" s="44"/>
       <c r="B157" s="36">
         <v>1978</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A158" s="43"/>
+      <c r="A158" s="44"/>
       <c r="B158" s="36">
         <v>1979</v>
       </c>
@@ -9293,7 +9335,7 @@
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A159" s="43"/>
+      <c r="A159" s="44"/>
       <c r="B159" s="36">
         <v>1980</v>
       </c>
@@ -9305,19 +9347,19 @@
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A160" s="43"/>
+      <c r="A160" s="44"/>
       <c r="B160" s="36">
         <v>1981</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A161" s="43"/>
+      <c r="A161" s="44"/>
       <c r="B161" s="36">
         <v>1982</v>
       </c>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A162" s="43"/>
+      <c r="A162" s="44"/>
       <c r="B162" s="36">
         <v>1983</v>
       </c>
@@ -9329,7 +9371,7 @@
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A163" s="43"/>
+      <c r="A163" s="44"/>
       <c r="B163" s="36">
         <v>1984</v>
       </c>
@@ -9338,7 +9380,7 @@
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A164" s="43"/>
+      <c r="A164" s="44"/>
       <c r="B164" s="36">
         <v>1985</v>
       </c>
@@ -9350,13 +9392,13 @@
       </c>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A165" s="43"/>
+      <c r="A165" s="44"/>
       <c r="B165" s="36">
         <v>1986</v>
       </c>
     </row>
     <row r="166" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A166" s="43"/>
+      <c r="A166" s="44"/>
       <c r="B166" s="36">
         <v>1987</v>
       </c>
@@ -9365,13 +9407,13 @@
       </c>
     </row>
     <row r="167" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="43"/>
+      <c r="A167" s="44"/>
       <c r="J167" s="31" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="168" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A168" s="43"/>
+      <c r="A168" s="44"/>
       <c r="B168" s="36">
         <v>1988</v>
       </c>
@@ -9383,7 +9425,7 @@
       </c>
     </row>
     <row r="169" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A169" s="43"/>
+      <c r="A169" s="44"/>
       <c r="B169" s="36">
         <v>1989</v>
       </c>
@@ -9395,7 +9437,7 @@
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A170" s="43"/>
+      <c r="A170" s="44"/>
       <c r="B170" s="36">
         <v>1990</v>
       </c>
@@ -9404,7 +9446,7 @@
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A171" s="43"/>
+      <c r="A171" s="44"/>
       <c r="B171" s="36">
         <v>1991</v>
       </c>
@@ -9413,7 +9455,7 @@
       </c>
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A172" s="43"/>
+      <c r="A172" s="44"/>
       <c r="B172" s="36">
         <v>1992</v>
       </c>
@@ -9425,13 +9467,13 @@
       </c>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A173" s="43"/>
+      <c r="A173" s="44"/>
       <c r="J173" s="31" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A174" s="43"/>
+      <c r="A174" s="44"/>
       <c r="B174" s="36">
         <v>1993</v>
       </c>
@@ -9440,17 +9482,17 @@
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A175" s="43"/>
+      <c r="A175" s="44"/>
       <c r="B175" s="36">
         <v>1994</v>
       </c>
-      <c r="K175" s="44" t="s">
+      <c r="K175" s="43" t="s">
         <v>263</v>
       </c>
-      <c r="L175" s="44"/>
+      <c r="L175" s="43"/>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A176" s="43"/>
+      <c r="A176" s="44"/>
       <c r="B176" s="36">
         <v>1995</v>
       </c>
@@ -9459,7 +9501,7 @@
       </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A177" s="43" t="s">
+      <c r="A177" s="44" t="s">
         <v>69</v>
       </c>
       <c r="B177" s="36">
@@ -9467,13 +9509,13 @@
       </c>
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A178" s="43"/>
+      <c r="A178" s="44"/>
       <c r="B178" s="36">
         <v>1997</v>
       </c>
     </row>
     <row r="179" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A179" s="43"/>
+      <c r="A179" s="44"/>
       <c r="B179" s="36">
         <v>1998</v>
       </c>
@@ -9485,7 +9527,7 @@
       </c>
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A180" s="43"/>
+      <c r="A180" s="44"/>
       <c r="B180" s="36">
         <v>1999</v>
       </c>
@@ -9494,13 +9536,13 @@
       </c>
     </row>
     <row r="181" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A181" s="43"/>
+      <c r="A181" s="44"/>
       <c r="K181" s="31" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="182" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A182" s="43"/>
+      <c r="A182" s="44"/>
       <c r="B182" s="36">
         <v>2000</v>
       </c>
@@ -9512,7 +9554,7 @@
       </c>
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A183" s="43"/>
+      <c r="A183" s="44"/>
       <c r="B183" s="36">
         <v>2001</v>
       </c>
@@ -9521,31 +9563,31 @@
       </c>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A184" s="43"/>
+      <c r="A184" s="44"/>
       <c r="B184" s="36">
         <v>2002</v>
       </c>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A185" s="43"/>
+      <c r="A185" s="44"/>
       <c r="B185" s="36">
         <v>2003</v>
       </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A186" s="43"/>
+      <c r="A186" s="44"/>
       <c r="B186" s="36">
         <v>2004</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A187" s="43"/>
+      <c r="A187" s="44"/>
       <c r="B187" s="36">
         <v>2005</v>
       </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A188" s="43" t="s">
+      <c r="A188" s="44" t="s">
         <v>70</v>
       </c>
       <c r="B188" s="36">
@@ -9553,25 +9595,25 @@
       </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A189" s="43"/>
+      <c r="A189" s="44"/>
       <c r="B189" s="36">
         <v>2007</v>
       </c>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A190" s="43"/>
+      <c r="A190" s="44"/>
       <c r="B190" s="36">
         <v>2008</v>
       </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A191" s="43"/>
+      <c r="A191" s="44"/>
       <c r="B191" s="36">
         <v>2009</v>
       </c>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A192" s="43"/>
+      <c r="A192" s="44"/>
       <c r="B192" s="36">
         <v>2010</v>
       </c>
@@ -9580,19 +9622,19 @@
       </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A193" s="43"/>
+      <c r="A193" s="44"/>
       <c r="B193" s="36">
         <v>2011</v>
       </c>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A194" s="43"/>
+      <c r="A194" s="44"/>
       <c r="B194" s="36">
         <v>2012</v>
       </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A195" s="43"/>
+      <c r="A195" s="44"/>
       <c r="B195" s="36">
         <v>2013</v>
       </c>
@@ -9601,7 +9643,7 @@
       </c>
     </row>
     <row r="196" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" s="43"/>
+      <c r="A196" s="44"/>
       <c r="B196" s="36">
         <v>2014</v>
       </c>
@@ -9613,7 +9655,7 @@
       </c>
     </row>
     <row r="197" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A197" s="43"/>
+      <c r="A197" s="44"/>
       <c r="B197" s="36">
         <v>2015</v>
       </c>
@@ -9622,13 +9664,13 @@
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A198" s="43"/>
+      <c r="A198" s="44"/>
       <c r="B198" s="36">
         <v>2016</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A199" s="43"/>
+      <c r="A199" s="44"/>
       <c r="B199" s="36">
         <v>2017</v>
       </c>
@@ -9637,7 +9679,7 @@
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A200" s="43"/>
+      <c r="A200" s="44"/>
       <c r="B200" s="36">
         <v>2018</v>
       </c>
@@ -9646,58 +9688,63 @@
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A201" s="43"/>
+      <c r="A201" s="44"/>
       <c r="B201" s="36">
         <v>2019</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A202" s="43"/>
+      <c r="A202" s="44"/>
       <c r="B202" s="36">
         <v>2020</v>
       </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A203" s="43"/>
+      <c r="A203" s="44"/>
       <c r="B203" s="36">
         <v>2021</v>
       </c>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A204" s="43"/>
+      <c r="A204" s="44"/>
       <c r="B204" s="36">
         <v>2022</v>
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A205" s="43"/>
+      <c r="A205" s="44"/>
       <c r="B205" s="36">
         <v>2023</v>
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A206" s="43"/>
+      <c r="A206" s="44"/>
       <c r="B206" s="36">
         <v>2024</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A207" s="43"/>
+      <c r="A207" s="44"/>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A208" s="43"/>
+      <c r="A208" s="44"/>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="43"/>
+      <c r="A209" s="44"/>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="43"/>
+      <c r="A210" s="44"/>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="43"/>
+      <c r="A211" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="A114:A126"/>
+    <mergeCell ref="A2:A53"/>
+    <mergeCell ref="A54:A76"/>
+    <mergeCell ref="A77:A113"/>
     <mergeCell ref="K175:L175"/>
     <mergeCell ref="A177:A187"/>
     <mergeCell ref="A188:A211"/>
@@ -9706,11 +9753,6 @@
     <mergeCell ref="A127:A148"/>
     <mergeCell ref="A149:A176"/>
     <mergeCell ref="B135:B138"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="A114:A126"/>
-    <mergeCell ref="A2:A53"/>
-    <mergeCell ref="A54:A76"/>
-    <mergeCell ref="A77:A113"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>